<commit_message>
Completed Screen Mockups and initial database design
</commit_message>
<xml_diff>
--- a/Documentation/DatabaseLayout.xlsx
+++ b/Documentation/DatabaseLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2f1d0a01d04997c5/Documents/GitHub/AndroidProject/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\OneDrive\Documents\GitHub\AndroidProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{F1BCB684-953A-4DA2-A103-808EB439D1D1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{D1AE9160-2E85-4512-B198-FC5FA248FA52}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{F1BCB684-953A-4DA2-A103-808EB439D1D1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{9C9D3C2F-5709-4639-A15E-D864849A9F44}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{A3491008-682C-4A1B-B406-E581513D469D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="2" xr2:uid="{A3491008-682C-4A1B-B406-E581513D469D}"/>
   </bookViews>
   <sheets>
     <sheet name="Engines" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>ESN</t>
   </si>
@@ -135,9 +135,6 @@
     <t>CyclesSinceNew</t>
   </si>
   <si>
-    <t>EngineConfiguration</t>
-  </si>
-  <si>
     <t>ExaustGasTemperature</t>
   </si>
   <si>
@@ -145,6 +142,15 @@
   </si>
   <si>
     <t>Operator</t>
+  </si>
+  <si>
+    <t>EngineDesignation</t>
+  </si>
+  <si>
+    <t>CurrentEGT Margin</t>
+  </si>
+  <si>
+    <t>Estimated Time To Shop Visit</t>
   </si>
 </sst>
 </file>
@@ -169,12 +175,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -192,8 +204,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EA5D77-CA9A-4C98-B8EC-999EB893EDC9}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,41 +560,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2FB098-AA34-4821-98BB-69EAF63C8A72}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -595,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2429EF05-D0B8-4D4E-9ECB-61CE41E92F3A}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1010,24 +1027,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D062DD-E530-4ECF-8566-24BD77CCF308}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1038,22 +1057,34 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" t="s">
-        <v>37</v>
+      <c r="M1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added dalog box for engine record
</commit_message>
<xml_diff>
--- a/Documentation/DatabaseLayout.xlsx
+++ b/Documentation/DatabaseLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\OneDrive\Documents\GitHub\AndroidProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{F1BCB684-953A-4DA2-A103-808EB439D1D1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{9C9D3C2F-5709-4639-A15E-D864849A9F44}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{F1BCB684-953A-4DA2-A103-808EB439D1D1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{A4120448-26F3-476A-94BD-10CA08004899}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="2" xr2:uid="{A3491008-682C-4A1B-B406-E581513D469D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{A3491008-682C-4A1B-B406-E581513D469D}"/>
   </bookViews>
   <sheets>
     <sheet name="Engines" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
   <si>
     <t>ESN</t>
   </si>
@@ -90,9 +90,6 @@
     <t>5B9</t>
   </si>
   <si>
-    <t>EGTMCentegrate Degrees</t>
-  </si>
-  <si>
     <t>CFM56-5B</t>
   </si>
   <si>
@@ -151,6 +148,12 @@
   </si>
   <si>
     <t>Estimated Time To Shop Visit</t>
+  </si>
+  <si>
+    <t>Red_line_temprature</t>
+  </si>
+  <si>
+    <t>cycles_per_degree</t>
   </si>
 </sst>
 </file>
@@ -526,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EA5D77-CA9A-4C98-B8EC-999EB893EDC9}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,10 +563,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2FB098-AA34-4821-98BB-69EAF63C8A72}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,35 +575,32 @@
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -610,10 +610,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2429EF05-D0B8-4D4E-9ECB-61CE41E92F3A}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -637,10 +637,13 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -651,10 +654,10 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -668,7 +671,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -682,7 +685,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -696,7 +699,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -710,7 +713,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -724,7 +727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -738,7 +741,7 @@
         <v>-22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -752,7 +755,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -766,7 +769,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -780,9 +783,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -794,9 +797,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -808,9 +811,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -822,9 +825,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -836,9 +839,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -852,7 +855,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -866,7 +869,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -880,7 +883,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -894,7 +897,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -908,10 +911,10 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21">
         <v>10</v>
@@ -919,10 +922,10 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22">
         <v>-3</v>
@@ -930,10 +933,10 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23">
         <v>-18</v>
@@ -941,10 +944,10 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24">
         <v>-26</v>
@@ -952,10 +955,10 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25">
         <v>20</v>
@@ -966,10 +969,10 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26">
         <v>22</v>
@@ -980,10 +983,10 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27">
         <v>24</v>
@@ -994,10 +997,10 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28">
         <v>26</v>
@@ -1008,10 +1011,10 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29">
         <v>27</v>
@@ -1029,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D062DD-E530-4ECF-8566-24BD77CCF308}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,7 +1046,7 @@
     <col min="10" max="10" width="21.85546875" customWidth="1"/>
     <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1060,31 +1063,31 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
       </c>
       <c r="G1" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
         <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Engine Inspection Record Class
</commit_message>
<xml_diff>
--- a/Documentation/DatabaseLayout.xlsx
+++ b/Documentation/DatabaseLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\OneDrive\Documents\GitHub\AndroidProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{F1BCB684-953A-4DA2-A103-808EB439D1D1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{A4120448-26F3-476A-94BD-10CA08004899}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{F1BCB684-953A-4DA2-A103-808EB439D1D1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{EE218FDF-1B69-439B-9600-2A02E7E7B783}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{A3491008-682C-4A1B-B406-E581513D469D}"/>
   </bookViews>
@@ -1033,7 +1033,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1071,7 @@
       <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>34</v>
       </c>
       <c r="I1" t="s">
@@ -1092,5 +1092,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>